<commit_message>
esc: usind md files to contain work
</commit_message>
<xml_diff>
--- a/earth_system_and_climate_4/term_1/practical_2/data/d-18O.xlsx
+++ b/earth_system_and_climate_4/term_1/practical_2/data/d-18O.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackycao/Documents/Projects/degree_level4/earth_system_and_climate_4/term_1/practical_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168207F2-0D6E-4642-90BA-421F13EB02FC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5E0EE5-B9CD-284E-83B1-580207EB52CD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13517,7 +13517,7 @@
   <dimension ref="B2:C2025"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>